<commit_message>
Work done over holidays
GUI Created - used IMGUI library
Gantt Chart updated
Enigma components created in blender
</commit_message>
<xml_diff>
--- a/Documentation/Minutes.xlsx
+++ b/Documentation/Minutes.xlsx
@@ -364,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,6 +471,22 @@
         <v>0.54166666666666663</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>41968</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>41976</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>